<commit_message>
Save the two Excel examples with JS manipulation
</commit_message>
<xml_diff>
--- a/JS_Excel_files/10_EntireShippingCosts/10_EntireShippingCosts_1.xlsx
+++ b/JS_Excel_files/10_EntireShippingCosts/10_EntireShippingCosts_1.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amilas_Windows_VM\Documents\SheetCoPilot\SheetCopilot\output_dir\10_EntireShippingCosts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amilas_Windows_VM\Documents\SheetCoPilot\SheetCopilot\JS_Excel_files\10_EntireShippingCosts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5E96A8-3E80-4D52-8E73-CB5B897684C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCF051F-45BB-418F-85F1-FC658C7BB663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13695" activeTab="1" xr2:uid="{134BE2BE-B2C4-40DC-9526-9AC5254CBFD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{134BE2BE-B2C4-40DC-9526-9AC5254CBFD7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$E$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -637,7 +637,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="919" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -656,10 +656,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEABFDF-C14A-42C4-A235-779488ABD940}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1447</v>
+      </c>
+      <c r="C2">
+        <v>1830</v>
+      </c>
+      <c r="D2">
+        <v>1686</v>
+      </c>
+      <c r="E2">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1405</v>
+      </c>
+      <c r="C3">
+        <v>1870</v>
+      </c>
+      <c r="D3">
+        <v>1715</v>
+      </c>
+      <c r="E3">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1440</v>
+      </c>
+      <c r="C4">
+        <v>1816</v>
+      </c>
+      <c r="D4">
+        <v>1702</v>
+      </c>
+      <c r="E4">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1435</v>
+      </c>
+      <c r="C5">
+        <v>1818</v>
+      </c>
+      <c r="D5">
+        <v>1706</v>
+      </c>
+      <c r="E5">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2277</v>
+      </c>
+      <c r="C6">
+        <v>743</v>
+      </c>
+      <c r="D6">
+        <v>373</v>
+      </c>
+      <c r="E6">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>796</v>
+      </c>
+      <c r="C7">
+        <v>2146</v>
+      </c>
+      <c r="D7">
+        <v>2299</v>
+      </c>
+      <c r="E7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>795</v>
+      </c>
+      <c r="C8">
+        <v>2165</v>
+      </c>
+      <c r="D8">
+        <v>2319</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1258</v>
+      </c>
+      <c r="C9">
+        <v>2124</v>
+      </c>
+      <c r="D9">
+        <v>1996</v>
+      </c>
+      <c r="E9">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>785</v>
+      </c>
+      <c r="C10">
+        <v>2155</v>
+      </c>
+      <c r="D10">
+        <v>2319</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7131FD02-5136-4587-8796-E5071711B6D9}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -1881,189 +2064,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFD67DF-A957-409F-BCE3-8927FC2C2F97}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1447</v>
-      </c>
-      <c r="C2">
-        <v>1830</v>
-      </c>
-      <c r="D2">
-        <v>1686</v>
-      </c>
-      <c r="E2">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1405</v>
-      </c>
-      <c r="C3">
-        <v>1870</v>
-      </c>
-      <c r="D3">
-        <v>1715</v>
-      </c>
-      <c r="E3">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1440</v>
-      </c>
-      <c r="C4">
-        <v>1816</v>
-      </c>
-      <c r="D4">
-        <v>1702</v>
-      </c>
-      <c r="E4">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1435</v>
-      </c>
-      <c r="C5">
-        <v>1818</v>
-      </c>
-      <c r="D5">
-        <v>1706</v>
-      </c>
-      <c r="E5">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2277</v>
-      </c>
-      <c r="C6">
-        <v>743</v>
-      </c>
-      <c r="D6">
-        <v>373</v>
-      </c>
-      <c r="E6">
-        <v>1955</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>796</v>
-      </c>
-      <c r="C7">
-        <v>2146</v>
-      </c>
-      <c r="D7">
-        <v>2299</v>
-      </c>
-      <c r="E7">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>795</v>
-      </c>
-      <c r="C8">
-        <v>2165</v>
-      </c>
-      <c r="D8">
-        <v>2319</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1258</v>
-      </c>
-      <c r="C9">
-        <v>2124</v>
-      </c>
-      <c r="D9">
-        <v>1996</v>
-      </c>
-      <c r="E9">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>785</v>
-      </c>
-      <c r="C10">
-        <v>2155</v>
-      </c>
-      <c r="D10">
-        <v>2319</v>
-      </c>
-      <c r="E10">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>